<commit_message>
Missing 5 bw_rt just 1
</commit_message>
<xml_diff>
--- a/coordinates_v2.xlsx
+++ b/coordinates_v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="48" windowWidth="22056" windowHeight="9552" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="48" windowWidth="22056" windowHeight="9552"/>
   </bookViews>
   <sheets>
     <sheet name="23" sheetId="1" r:id="rId1"/>
@@ -479,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1384,8 +1384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>

<commit_message>
Tested a6300 LL ev0
</commit_message>
<xml_diff>
--- a/coordinates_v2.xlsx
+++ b/coordinates_v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="48" windowWidth="22056" windowHeight="9552"/>
+    <workbookView xWindow="480" yWindow="48" windowWidth="22056" windowHeight="9552" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="23" sheetId="1" r:id="rId1"/>
@@ -479,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -517,16 +517,16 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>7.5</v>
+        <v>6.5</v>
       </c>
       <c r="D2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -536,19 +536,19 @@
       </c>
       <c r="H2">
         <f>B2-$G$2</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I2">
         <f>C2-$G$2</f>
-        <v>6.5</v>
+        <v>5.5</v>
       </c>
       <c r="J2">
         <f>D2+$G$2</f>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K2">
         <f>E2+$G$2</f>
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -556,35 +556,35 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C3">
-        <v>5.5</v>
+        <v>4.5</v>
       </c>
       <c r="D3">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="E3">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F3" t="s">
         <v>1</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H18" si="0">B3-$G$2</f>
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I18" si="1">C3-$G$2</f>
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J18" si="2">D3+$G$2</f>
-        <v>544</v>
+        <f t="shared" ref="J3:J9" si="2">D3+$G$2</f>
+        <v>545</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K18" si="3">E3+$G$2</f>
-        <v>53</v>
+        <f t="shared" ref="K3:K9" si="3">E3+$G$2</f>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -592,35 +592,35 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>314.67</v>
+        <v>313.67</v>
       </c>
       <c r="D4">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E4">
-        <v>361.17</v>
+        <v>362.17</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I4">
         <f t="shared" si="1"/>
-        <v>313.67</v>
+        <v>312.67</v>
       </c>
       <c r="J4">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K4">
         <f t="shared" si="3"/>
-        <v>362.17</v>
+        <v>363.17</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -628,35 +628,35 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C5">
-        <v>307.67</v>
+        <v>306.67</v>
       </c>
       <c r="D5">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="E5">
-        <v>354.17</v>
+        <v>355.17</v>
       </c>
       <c r="F5" t="s">
         <v>14</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
-        <v>306.67</v>
+        <v>305.67</v>
       </c>
       <c r="J5">
         <f t="shared" si="2"/>
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="K5">
         <f t="shared" si="3"/>
-        <v>355.17</v>
+        <v>356.17</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -664,35 +664,35 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>244.5</v>
+        <v>243.5</v>
       </c>
       <c r="C6">
-        <v>129.35499999999999</v>
+        <v>128.35499999999999</v>
       </c>
       <c r="D6">
-        <v>269.5</v>
+        <v>270.5</v>
       </c>
       <c r="E6">
-        <v>175.83500000000001</v>
+        <v>176.83500000000001</v>
       </c>
       <c r="F6" t="s">
         <v>15</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>243.5</v>
+        <v>242.5</v>
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
-        <v>128.35499999999999</v>
+        <v>127.35499999999999</v>
       </c>
       <c r="J6">
         <f t="shared" si="2"/>
-        <v>270.5</v>
+        <v>271.5</v>
       </c>
       <c r="K6">
         <f t="shared" si="3"/>
-        <v>176.83500000000001</v>
+        <v>177.83500000000001</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -700,35 +700,35 @@
         <v>16</v>
       </c>
       <c r="B7">
-        <v>280.5</v>
+        <v>279.5</v>
       </c>
       <c r="C7">
-        <v>129.35499999999999</v>
+        <v>128.35499999999999</v>
       </c>
       <c r="D7">
-        <v>305.5</v>
+        <v>306.5</v>
       </c>
       <c r="E7">
-        <v>175.83500000000001</v>
+        <v>176.83500000000001</v>
       </c>
       <c r="F7" t="s">
         <v>17</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>279.5</v>
+        <v>278.5</v>
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
-        <v>128.35499999999999</v>
+        <v>127.35499999999999</v>
       </c>
       <c r="J7">
         <f t="shared" si="2"/>
-        <v>306.5</v>
+        <v>307.5</v>
       </c>
       <c r="K7">
         <f t="shared" si="3"/>
-        <v>176.83500000000001</v>
+        <v>177.83500000000001</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -736,35 +736,35 @@
         <v>21</v>
       </c>
       <c r="B8">
-        <v>280.5</v>
+        <v>279.5</v>
       </c>
       <c r="C8">
-        <v>190.83500000000001</v>
+        <v>189.83500000000001</v>
       </c>
       <c r="D8">
-        <v>305.5</v>
+        <v>306.5</v>
       </c>
       <c r="E8">
-        <v>237.33500000000001</v>
+        <v>238.33500000000001</v>
       </c>
       <c r="F8" t="s">
         <v>19</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>279.5</v>
+        <v>278.5</v>
       </c>
       <c r="I8">
         <f t="shared" si="1"/>
-        <v>189.83500000000001</v>
+        <v>188.83500000000001</v>
       </c>
       <c r="J8">
         <f t="shared" si="2"/>
-        <v>306.5</v>
+        <v>307.5</v>
       </c>
       <c r="K8">
         <f t="shared" si="3"/>
-        <v>238.33500000000001</v>
+        <v>239.33500000000001</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -772,35 +772,35 @@
         <v>20</v>
       </c>
       <c r="B9">
-        <v>244.5</v>
+        <v>243.5</v>
       </c>
       <c r="C9">
-        <v>190.83500000000001</v>
+        <v>189.83500000000001</v>
       </c>
       <c r="D9">
-        <v>269.5</v>
+        <v>270.5</v>
       </c>
       <c r="E9">
-        <v>237.33500000000001</v>
+        <v>238.33500000000001</v>
       </c>
       <c r="F9" t="s">
         <v>18</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>243.5</v>
+        <v>242.5</v>
       </c>
       <c r="I9">
         <f t="shared" si="1"/>
-        <v>189.83500000000001</v>
+        <v>188.83500000000001</v>
       </c>
       <c r="J9">
         <f t="shared" si="2"/>
-        <v>270.5</v>
+        <v>271.5</v>
       </c>
       <c r="K9">
         <f t="shared" si="3"/>
-        <v>238.33500000000001</v>
+        <v>239.33500000000001</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -822,22 +822,6 @@
       <c r="F10" t="s">
         <v>23</v>
       </c>
-      <c r="H10">
-        <f t="shared" si="0"/>
-        <v>74.055499999999995</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="2"/>
-        <v>256.05549999999999</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="3"/>
-        <v>78</v>
-      </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
@@ -858,22 +842,6 @@
       <c r="F11" t="s">
         <v>24</v>
       </c>
-      <c r="H11">
-        <f t="shared" si="0"/>
-        <v>293.44450000000001</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="2"/>
-        <v>475.44450000000001</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="3"/>
-        <v>78</v>
-      </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
@@ -894,22 +862,6 @@
       <c r="F12" t="s">
         <v>25</v>
       </c>
-      <c r="H12">
-        <f t="shared" si="0"/>
-        <v>74.055499999999995</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="1"/>
-        <v>288.66699999999997</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="2"/>
-        <v>256.05549999999999</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="3"/>
-        <v>366.66699999999997</v>
-      </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" t="s">
@@ -930,22 +882,6 @@
       <c r="F13" t="s">
         <v>26</v>
       </c>
-      <c r="H13">
-        <f t="shared" si="0"/>
-        <v>293.44450000000001</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="1"/>
-        <v>288.66699999999997</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="2"/>
-        <v>475.44450000000001</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="3"/>
-        <v>366.66699999999997</v>
-      </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" t="s">
@@ -966,22 +902,6 @@
       <c r="F14" t="s">
         <v>32</v>
       </c>
-      <c r="H14">
-        <f t="shared" si="0"/>
-        <v>315.6825</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="1"/>
-        <v>86.5762</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="2"/>
-        <v>489.625</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="3"/>
-        <v>175.5762</v>
-      </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
@@ -1002,22 +922,6 @@
       <c r="F15" t="s">
         <v>33</v>
       </c>
-      <c r="H15">
-        <f t="shared" si="0"/>
-        <v>315.6825</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="1"/>
-        <v>195.07810000000001</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="2"/>
-        <v>489.625</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="3"/>
-        <v>284.07810000000001</v>
-      </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
@@ -1038,22 +942,6 @@
       <c r="F16" t="s">
         <v>34</v>
       </c>
-      <c r="H16">
-        <f t="shared" si="0"/>
-        <v>36.355899999999998</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="1"/>
-        <v>79.174499999999995</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="2"/>
-        <v>236.35589999999999</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="3"/>
-        <v>119.17449999999999</v>
-      </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
@@ -1074,22 +962,6 @@
       <c r="F17" t="s">
         <v>35</v>
       </c>
-      <c r="H17">
-        <f t="shared" si="0"/>
-        <v>76.355900000000005</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="1"/>
-        <v>193.45590000000001</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="2"/>
-        <v>196.35589999999999</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="3"/>
-        <v>253.45590000000001</v>
-      </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" t="s">
@@ -1110,32 +982,68 @@
       <c r="F18" t="s">
         <v>39</v>
       </c>
-      <c r="H18">
-        <f t="shared" si="0"/>
-        <v>68.355199999999996</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="1"/>
-        <v>127.75749999999999</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="2"/>
-        <v>204.3552</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="3"/>
-        <v>163.75749999999999</v>
-      </c>
     </row>
     <row r="21" spans="1:11">
       <c r="F21" t="s">
         <v>18</v>
       </c>
+      <c r="H21">
+        <v>5</v>
+      </c>
+      <c r="I21">
+        <v>7.5</v>
+      </c>
+      <c r="J21">
+        <v>30</v>
+      </c>
+      <c r="K21">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="H22">
+        <v>518</v>
+      </c>
+      <c r="I22">
+        <v>5.5</v>
+      </c>
+      <c r="J22">
+        <v>543</v>
+      </c>
+      <c r="K22">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="H23">
+        <v>7</v>
+      </c>
+      <c r="I23">
+        <v>314.67</v>
+      </c>
+      <c r="J23">
+        <v>32</v>
+      </c>
+      <c r="K23">
+        <v>361.17</v>
+      </c>
     </row>
     <row r="24" spans="1:11">
       <c r="B24" t="s">
         <v>42</v>
       </c>
+      <c r="H24">
+        <v>519</v>
+      </c>
+      <c r="I24">
+        <v>307.67</v>
+      </c>
+      <c r="J24">
+        <v>544</v>
+      </c>
+      <c r="K24">
+        <v>354.17</v>
+      </c>
     </row>
     <row r="25" spans="1:11">
       <c r="B25">
@@ -1150,6 +1058,18 @@
       <c r="E25">
         <v>53</v>
       </c>
+      <c r="H25">
+        <v>244.5</v>
+      </c>
+      <c r="I25">
+        <v>129.35499999999999</v>
+      </c>
+      <c r="J25">
+        <v>269.5</v>
+      </c>
+      <c r="K25">
+        <v>175.83500000000001</v>
+      </c>
     </row>
     <row r="26" spans="1:11">
       <c r="B26">
@@ -1164,6 +1084,18 @@
       <c r="E26">
         <v>53</v>
       </c>
+      <c r="H26">
+        <v>280.5</v>
+      </c>
+      <c r="I26">
+        <v>129.35499999999999</v>
+      </c>
+      <c r="J26">
+        <v>305.5</v>
+      </c>
+      <c r="K26">
+        <v>175.83500000000001</v>
+      </c>
     </row>
     <row r="27" spans="1:11">
       <c r="B27">
@@ -1178,6 +1110,18 @@
       <c r="E27">
         <v>358.17</v>
       </c>
+      <c r="H27">
+        <v>280.5</v>
+      </c>
+      <c r="I27">
+        <v>190.83500000000001</v>
+      </c>
+      <c r="J27">
+        <v>305.5</v>
+      </c>
+      <c r="K27">
+        <v>237.33500000000001</v>
+      </c>
     </row>
     <row r="28" spans="1:11">
       <c r="B28">
@@ -1191,6 +1135,18 @@
       </c>
       <c r="E28">
         <v>358.17</v>
+      </c>
+      <c r="H28">
+        <v>244.5</v>
+      </c>
+      <c r="I28">
+        <v>190.83500000000001</v>
+      </c>
+      <c r="J28">
+        <v>269.5</v>
+      </c>
+      <c r="K28">
+        <v>237.33500000000001</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1384,8 +1340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1421,16 +1377,16 @@
         <v>8</v>
       </c>
       <c r="B2" s="1">
-        <v>5.5000000000000036</v>
+        <v>4.5000000000000036</v>
       </c>
       <c r="C2" s="1">
-        <v>7.5</v>
+        <v>6.5</v>
       </c>
       <c r="D2" s="1">
-        <v>30.500000000000004</v>
+        <v>31.500000000000004</v>
       </c>
       <c r="E2" s="1">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -1440,19 +1396,19 @@
       </c>
       <c r="H2">
         <f>B2-$G$2</f>
-        <v>4.5000000000000036</v>
+        <v>3.5000000000000036</v>
       </c>
       <c r="I2">
         <f>C2-$G$2</f>
-        <v>6.5</v>
+        <v>5.5</v>
       </c>
       <c r="J2">
         <f>D2+$G$2</f>
-        <v>31.500000000000004</v>
+        <v>32.5</v>
       </c>
       <c r="K2">
         <f>E2+$G$2</f>
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1460,35 +1416,35 @@
         <v>9</v>
       </c>
       <c r="B3" s="1">
-        <v>458.38900000000001</v>
+        <v>457.38900000000001</v>
       </c>
       <c r="C3" s="1">
-        <v>7.5</v>
+        <v>6.5</v>
       </c>
       <c r="D3" s="1">
-        <v>483.38899999999995</v>
+        <v>484.38899999999995</v>
       </c>
       <c r="E3" s="1">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F3" t="s">
         <v>1</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H18" si="0">B3-$G$2</f>
-        <v>457.38900000000001</v>
+        <v>456.38900000000001</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I18" si="1">C3-$G$2</f>
-        <v>6.5</v>
+        <v>5.5</v>
       </c>
       <c r="J3">
         <f t="shared" ref="J3:J18" si="2">D3+$G$2</f>
-        <v>484.38899999999995</v>
+        <v>485.38899999999995</v>
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K18" si="3">E3+$G$2</f>
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1496,35 +1452,35 @@
         <v>10</v>
       </c>
       <c r="B4" s="1">
-        <v>5.5000000000000036</v>
+        <v>4.5000000000000036</v>
       </c>
       <c r="C4" s="1">
-        <v>312.67</v>
+        <v>311.67</v>
       </c>
       <c r="D4" s="1">
-        <v>30.500000000000004</v>
+        <v>31.500000000000004</v>
       </c>
       <c r="E4" s="1">
-        <v>359.17</v>
+        <v>360.17</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>4.5000000000000036</v>
+        <v>3.5000000000000036</v>
       </c>
       <c r="I4">
         <f t="shared" si="1"/>
-        <v>311.67</v>
+        <v>310.67</v>
       </c>
       <c r="J4">
         <f t="shared" si="2"/>
-        <v>31.500000000000004</v>
+        <v>32.5</v>
       </c>
       <c r="K4">
         <f t="shared" si="3"/>
-        <v>360.17</v>
+        <v>361.17</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1532,35 +1488,35 @@
         <v>11</v>
       </c>
       <c r="B5" s="1">
-        <v>458.38900000000001</v>
+        <v>457.38900000000001</v>
       </c>
       <c r="C5" s="1">
-        <v>312.67</v>
+        <v>311.67</v>
       </c>
       <c r="D5" s="1">
-        <v>483.38899999999995</v>
+        <v>484.38899999999995</v>
       </c>
       <c r="E5" s="1">
-        <v>359.17</v>
+        <v>360.17</v>
       </c>
       <c r="F5" t="s">
         <v>14</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>457.38900000000001</v>
+        <v>456.38900000000001</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
-        <v>311.67</v>
+        <v>310.67</v>
       </c>
       <c r="J5">
         <f t="shared" si="2"/>
-        <v>484.38899999999995</v>
+        <v>485.38899999999995</v>
       </c>
       <c r="K5">
         <f t="shared" si="3"/>
-        <v>360.17</v>
+        <v>361.17</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1568,35 +1524,35 @@
         <v>12</v>
       </c>
       <c r="B6" s="1">
-        <v>213.94450000000001</v>
+        <v>212.94450000000001</v>
       </c>
       <c r="C6" s="1">
-        <v>129.35499999999999</v>
+        <v>128.35499999999999</v>
       </c>
       <c r="D6" s="1">
-        <v>238.94450000000001</v>
+        <v>239.94450000000001</v>
       </c>
       <c r="E6" s="1">
-        <v>175.83500000000001</v>
+        <v>176.83500000000001</v>
       </c>
       <c r="F6" t="s">
         <v>15</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>212.94450000000001</v>
+        <v>211.94450000000001</v>
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
-        <v>128.35499999999999</v>
+        <v>127.35499999999999</v>
       </c>
       <c r="J6">
         <f t="shared" si="2"/>
-        <v>239.94450000000001</v>
+        <v>240.94450000000001</v>
       </c>
       <c r="K6">
         <f t="shared" si="3"/>
-        <v>176.83500000000001</v>
+        <v>177.83500000000001</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1604,35 +1560,35 @@
         <v>16</v>
       </c>
       <c r="B7" s="1">
-        <v>249.94450000000001</v>
+        <v>248.94450000000001</v>
       </c>
       <c r="C7" s="1">
-        <v>129.35499999999999</v>
+        <v>128.35499999999999</v>
       </c>
       <c r="D7" s="1">
-        <v>274.94450000000001</v>
+        <v>275.94450000000001</v>
       </c>
       <c r="E7" s="1">
-        <v>175.83500000000001</v>
+        <v>176.83500000000001</v>
       </c>
       <c r="F7" t="s">
         <v>17</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>248.94450000000001</v>
+        <v>247.94450000000001</v>
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
-        <v>128.35499999999999</v>
+        <v>127.35499999999999</v>
       </c>
       <c r="J7">
         <f t="shared" si="2"/>
-        <v>275.94450000000001</v>
+        <v>276.94450000000001</v>
       </c>
       <c r="K7">
         <f t="shared" si="3"/>
-        <v>176.83500000000001</v>
+        <v>177.83500000000001</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1640,35 +1596,35 @@
         <v>21</v>
       </c>
       <c r="B8" s="1">
-        <v>249.94450000000001</v>
+        <v>248.94450000000001</v>
       </c>
       <c r="C8" s="1">
-        <v>190.83500000000001</v>
+        <v>189.83500000000001</v>
       </c>
       <c r="D8" s="1">
-        <v>274.94450000000001</v>
+        <v>275.94450000000001</v>
       </c>
       <c r="E8" s="1">
-        <v>237.33500000000001</v>
+        <v>238.33500000000001</v>
       </c>
       <c r="F8" t="s">
         <v>19</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>248.94450000000001</v>
+        <v>247.94450000000001</v>
       </c>
       <c r="I8">
         <f t="shared" si="1"/>
-        <v>189.83500000000001</v>
+        <v>188.83500000000001</v>
       </c>
       <c r="J8">
         <f t="shared" si="2"/>
-        <v>275.94450000000001</v>
+        <v>276.94450000000001</v>
       </c>
       <c r="K8">
         <f t="shared" si="3"/>
-        <v>238.33500000000001</v>
+        <v>239.33500000000001</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1676,35 +1632,35 @@
         <v>20</v>
       </c>
       <c r="B9" s="1">
-        <v>213.94450000000001</v>
+        <v>212.94450000000001</v>
       </c>
       <c r="C9" s="1">
-        <v>190.83500000000001</v>
+        <v>189.83500000000001</v>
       </c>
       <c r="D9" s="1">
-        <v>238.94450000000001</v>
+        <v>239.94450000000001</v>
       </c>
       <c r="E9" s="1">
-        <v>237.33500000000001</v>
+        <v>238.33500000000001</v>
       </c>
       <c r="F9" t="s">
         <v>18</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>212.94450000000001</v>
+        <v>211.94450000000001</v>
       </c>
       <c r="I9">
         <f t="shared" si="1"/>
-        <v>189.83500000000001</v>
+        <v>188.83500000000001</v>
       </c>
       <c r="J9">
         <f t="shared" si="2"/>
-        <v>239.94450000000001</v>
+        <v>240.94450000000001</v>
       </c>
       <c r="K9">
         <f t="shared" si="3"/>
-        <v>238.33500000000001</v>
+        <v>239.33500000000001</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -2057,6 +2013,18 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
+      <c r="H24" s="1">
+        <v>5.5000000000000036</v>
+      </c>
+      <c r="I24" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="J24" s="1">
+        <v>30.500000000000004</v>
+      </c>
+      <c r="K24" s="1">
+        <v>54</v>
+      </c>
     </row>
     <row r="25" spans="1:11">
       <c r="B25" s="1" t="s">
@@ -2065,6 +2033,18 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
+      <c r="H25" s="1">
+        <v>458.38900000000001</v>
+      </c>
+      <c r="I25" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="J25" s="1">
+        <v>483.38899999999995</v>
+      </c>
+      <c r="K25" s="1">
+        <v>54</v>
+      </c>
     </row>
     <row r="26" spans="1:11">
       <c r="B26" s="1">
@@ -2079,6 +2059,18 @@
       <c r="E26" s="1">
         <v>53</v>
       </c>
+      <c r="H26" s="1">
+        <v>5.5000000000000036</v>
+      </c>
+      <c r="I26" s="1">
+        <v>312.67</v>
+      </c>
+      <c r="J26" s="1">
+        <v>30.500000000000004</v>
+      </c>
+      <c r="K26" s="1">
+        <v>359.17</v>
+      </c>
     </row>
     <row r="27" spans="1:11">
       <c r="B27" s="1">
@@ -2093,6 +2085,18 @@
       <c r="E27" s="1">
         <v>53</v>
       </c>
+      <c r="H27" s="1">
+        <v>458.38900000000001</v>
+      </c>
+      <c r="I27" s="1">
+        <v>312.67</v>
+      </c>
+      <c r="J27" s="1">
+        <v>483.38899999999995</v>
+      </c>
+      <c r="K27" s="1">
+        <v>359.17</v>
+      </c>
     </row>
     <row r="28" spans="1:11">
       <c r="B28" s="1">
@@ -2107,6 +2111,18 @@
       <c r="E28" s="1">
         <v>358.17</v>
       </c>
+      <c r="H28" s="1">
+        <v>213.94450000000001</v>
+      </c>
+      <c r="I28" s="1">
+        <v>129.35499999999999</v>
+      </c>
+      <c r="J28" s="1">
+        <v>238.94450000000001</v>
+      </c>
+      <c r="K28" s="1">
+        <v>175.83500000000001</v>
+      </c>
     </row>
     <row r="29" spans="1:11">
       <c r="B29" s="1">
@@ -2121,6 +2137,18 @@
       <c r="E29" s="1">
         <v>358.17</v>
       </c>
+      <c r="H29" s="1">
+        <v>249.94450000000001</v>
+      </c>
+      <c r="I29" s="1">
+        <v>129.35499999999999</v>
+      </c>
+      <c r="J29" s="1">
+        <v>274.94450000000001</v>
+      </c>
+      <c r="K29" s="1">
+        <v>175.83500000000001</v>
+      </c>
     </row>
     <row r="30" spans="1:11">
       <c r="B30" s="1">
@@ -2135,6 +2163,18 @@
       <c r="E30" s="1">
         <v>174.83500000000001</v>
       </c>
+      <c r="H30" s="1">
+        <v>249.94450000000001</v>
+      </c>
+      <c r="I30" s="1">
+        <v>190.83500000000001</v>
+      </c>
+      <c r="J30" s="1">
+        <v>274.94450000000001</v>
+      </c>
+      <c r="K30" s="1">
+        <v>237.33500000000001</v>
+      </c>
     </row>
     <row r="31" spans="1:11">
       <c r="B31" s="1">
@@ -2148,6 +2188,18 @@
       </c>
       <c r="E31" s="1">
         <v>174.83500000000001</v>
+      </c>
+      <c r="H31" s="1">
+        <v>213.94450000000001</v>
+      </c>
+      <c r="I31" s="1">
+        <v>190.83500000000001</v>
+      </c>
+      <c r="J31" s="1">
+        <v>238.94450000000001</v>
+      </c>
+      <c r="K31" s="1">
+        <v>237.33500000000001</v>
       </c>
     </row>
     <row r="32" spans="1:11">

</xml_diff>